<commit_message>
Debugged, develop image button and floorplan+schedule
</commit_message>
<xml_diff>
--- a/Web Design/App Dev Gantt.xlsx
+++ b/Web Design/App Dev Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{DE015C25-931E-4804-BE1F-9D49EF2A7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27733204-35E4-4B1E-B5F6-F1758E5705DB}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{DE015C25-931E-4804-BE1F-9D49EF2A7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{127FD6B1-BADB-4287-B1A5-1E7084399816}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>TB W3</t>
+  </si>
+  <si>
+    <t>T3 W2</t>
+  </si>
+  <si>
+    <t>T3 W3</t>
+  </si>
+  <si>
+    <t>T3 W4</t>
+  </si>
+  <si>
+    <t>T3 W5</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1136,7 +1148,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2" s="13"/>
       <c r="K2" s="29" t="s">
@@ -1229,16 +1241,16 @@
         <v>44</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
@@ -1358,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5" s="8">
         <v>0.75</v>
@@ -1418,10 +1430,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" s="8">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1438,10 +1450,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" s="8">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>